<commit_message>
update test with improved code
</commit_message>
<xml_diff>
--- a/example_files/dump_of_all_notes.xlsx
+++ b/example_files/dump_of_all_notes.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="41">
   <si>
     <t>Date</t>
   </si>
@@ -144,7 +144,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,13 +155,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -173,13 +190,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -469,13 +496,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -486,7 +513,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -497,7 +524,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -508,7 +535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -519,7 +546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -529,31 +556,31 @@
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <f>IF(SUM($B$3:$C$3)&gt;0,SUM($B$3:$C$3),1)</f>
         <v>0</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <f>IF(SUM($B$4:$C$4)&gt;0,SUM($B$4:$C$4),1)</f>
         <v>0</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <f>IF(SUM($B$5:$C$5)&gt;0,SUM($B$5:$C$5),1)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="E6" t="s">
+    <row r="6" spans="1:8">
+      <c r="F6" t="s">
         <v>13</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>14</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -563,20 +590,23 @@
       <c r="C7">
         <v>3</v>
       </c>
-      <c r="E7">
-        <f>SUMPRODUCT($B$3:$C$3, B7:C7)/E$5</f>
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <f>SUMPRODUCT($B$4:$C$4, B7:C7)/F$5</f>
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <f>SUMPRODUCT($B$5:$C$5, B7:C7)/G$5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="1">
+        <f>SUMPRODUCT($B$3:$C$3, B7:C7)/F$5</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <f>SUMPRODUCT($B$4:$C$4, B7:C7)/G$5</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <f>SUMPRODUCT($B$5:$C$5, B7:C7)/H$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -586,20 +616,23 @@
       <c r="C8">
         <v>4.5</v>
       </c>
-      <c r="E8">
-        <f>SUMPRODUCT($B$3:$C$3, B8:C8)/E$5</f>
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <f>SUMPRODUCT($B$4:$C$4, B8:C8)/F$5</f>
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <f>SUMPRODUCT($B$5:$C$5, B8:C8)/G$5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="1">
+        <f>SUMPRODUCT($B$3:$C$3, B8:C8)/F$5</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <f>SUMPRODUCT($B$4:$C$4, B8:C8)/G$5</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <f>SUMPRODUCT($B$5:$C$5, B8:C8)/H$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -609,20 +642,23 @@
       <c r="C9">
         <v>3</v>
       </c>
-      <c r="E9">
-        <f>SUMPRODUCT($B$3:$C$3, B9:C9)/E$5</f>
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <f>SUMPRODUCT($B$4:$C$4, B9:C9)/F$5</f>
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <f>SUMPRODUCT($B$5:$C$5, B9:C9)/G$5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="1">
+        <f>SUMPRODUCT($B$3:$C$3, B9:C9)/F$5</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <f>SUMPRODUCT($B$4:$C$4, B9:C9)/G$5</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <f>SUMPRODUCT($B$5:$C$5, B9:C9)/H$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -632,33 +668,42 @@
       <c r="C10">
         <v>4</v>
       </c>
-      <c r="E10">
-        <f>SUMPRODUCT($B$3:$C$3, B10:C10)/E$5</f>
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <f>SUMPRODUCT($B$4:$C$4, B10:C10)/F$5</f>
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <f>SUMPRODUCT($B$5:$C$5, B10:C10)/G$5</f>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="1">
+        <f>SUMPRODUCT($B$3:$C$3, B10:C10)/F$5</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <f>SUMPRODUCT($B$4:$C$4, B10:C10)/G$5</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <f>SUMPRODUCT($B$5:$C$5, B10:C10)/H$5</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="F7:H10">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
+      <formula>-100.0</formula>
+      <formula>3.945</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -666,7 +711,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -674,7 +719,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -682,7 +727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -690,429 +735,573 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <f>IF(SUM($B$3)&gt;0,SUM($B$3),1)</f>
         <v>0</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <f>IF(SUM($B$4)&gt;0,SUM($B$4),1)</f>
         <v>0</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <f>IF(SUM($B$5)&gt;0,SUM($B$5),1)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="D6" t="s">
+    <row r="6" spans="1:7">
+      <c r="E6" t="s">
         <v>13</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>14</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>18</v>
       </c>
-      <c r="D7">
-        <f>SUMPRODUCT($B$3, B7)/D$5</f>
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <f>SUMPRODUCT($B$4, B7)/E$5</f>
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <f>SUMPRODUCT($B$5, B7)/F$5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="B7" s="2">
+        <v>-100</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="1">
+        <f>SUMPRODUCT($B$3, B7)/E$5</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <f>SUMPRODUCT($B$4, B7)/F$5</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <f>SUMPRODUCT($B$5, B7)/G$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>19</v>
       </c>
-      <c r="D8">
-        <f>SUMPRODUCT($B$3, B8)/D$5</f>
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <f>SUMPRODUCT($B$4, B8)/E$5</f>
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <f>SUMPRODUCT($B$5, B8)/F$5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="B8" s="2">
+        <v>-100</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="1">
+        <f>SUMPRODUCT($B$3, B8)/E$5</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <f>SUMPRODUCT($B$4, B8)/F$5</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <f>SUMPRODUCT($B$5, B8)/G$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>20</v>
       </c>
-      <c r="D9">
-        <f>SUMPRODUCT($B$3, B9)/D$5</f>
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <f>SUMPRODUCT($B$4, B9)/E$5</f>
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <f>SUMPRODUCT($B$5, B9)/F$5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="B9" s="2">
+        <v>-100</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="1">
+        <f>SUMPRODUCT($B$3, B9)/E$5</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <f>SUMPRODUCT($B$4, B9)/F$5</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <f>SUMPRODUCT($B$5, B9)/G$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>21</v>
       </c>
-      <c r="D10">
-        <f>SUMPRODUCT($B$3, B10)/D$5</f>
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <f>SUMPRODUCT($B$4, B10)/E$5</f>
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <f>SUMPRODUCT($B$5, B10)/F$5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="B10" s="2">
+        <v>-100</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="1">
+        <f>SUMPRODUCT($B$3, B10)/E$5</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <f>SUMPRODUCT($B$4, B10)/F$5</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <f>SUMPRODUCT($B$5, B10)/G$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>22</v>
       </c>
-      <c r="D11">
-        <f>SUMPRODUCT($B$3, B11)/D$5</f>
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <f>SUMPRODUCT($B$4, B11)/E$5</f>
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <f>SUMPRODUCT($B$5, B11)/F$5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="B11" s="2">
+        <v>-100</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="1">
+        <f>SUMPRODUCT($B$3, B11)/E$5</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <f>SUMPRODUCT($B$4, B11)/F$5</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <f>SUMPRODUCT($B$5, B11)/G$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>23</v>
       </c>
-      <c r="D12">
-        <f>SUMPRODUCT($B$3, B12)/D$5</f>
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <f>SUMPRODUCT($B$4, B12)/E$5</f>
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <f>SUMPRODUCT($B$5, B12)/F$5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="B12" s="2">
+        <v>-100</v>
+      </c>
+      <c r="D12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="1">
+        <f>SUMPRODUCT($B$3, B12)/E$5</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <f>SUMPRODUCT($B$4, B12)/F$5</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <f>SUMPRODUCT($B$5, B12)/G$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>24</v>
       </c>
-      <c r="D13">
-        <f>SUMPRODUCT($B$3, B13)/D$5</f>
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <f>SUMPRODUCT($B$4, B13)/E$5</f>
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <f>SUMPRODUCT($B$5, B13)/F$5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="B13" s="2">
+        <v>-100</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="1">
+        <f>SUMPRODUCT($B$3, B13)/E$5</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <f>SUMPRODUCT($B$4, B13)/F$5</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
+        <f>SUMPRODUCT($B$5, B13)/G$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>25</v>
       </c>
-      <c r="D14">
-        <f>SUMPRODUCT($B$3, B14)/D$5</f>
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <f>SUMPRODUCT($B$4, B14)/E$5</f>
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <f>SUMPRODUCT($B$5, B14)/F$5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="B14" s="2">
+        <v>-100</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="1">
+        <f>SUMPRODUCT($B$3, B14)/E$5</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <f>SUMPRODUCT($B$4, B14)/F$5</f>
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <f>SUMPRODUCT($B$5, B14)/G$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>26</v>
       </c>
-      <c r="D15">
-        <f>SUMPRODUCT($B$3, B15)/D$5</f>
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <f>SUMPRODUCT($B$4, B15)/E$5</f>
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <f>SUMPRODUCT($B$5, B15)/F$5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="B15" s="2">
+        <v>-100</v>
+      </c>
+      <c r="D15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="1">
+        <f>SUMPRODUCT($B$3, B15)/E$5</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <f>SUMPRODUCT($B$4, B15)/F$5</f>
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <f>SUMPRODUCT($B$5, B15)/G$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>27</v>
       </c>
-      <c r="D16">
-        <f>SUMPRODUCT($B$3, B16)/D$5</f>
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <f>SUMPRODUCT($B$4, B16)/E$5</f>
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <f>SUMPRODUCT($B$5, B16)/F$5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="B16" s="2">
+        <v>-100</v>
+      </c>
+      <c r="D16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="1">
+        <f>SUMPRODUCT($B$3, B16)/E$5</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="1">
+        <f>SUMPRODUCT($B$4, B16)/F$5</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <f>SUMPRODUCT($B$5, B16)/G$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>28</v>
       </c>
-      <c r="D17">
-        <f>SUMPRODUCT($B$3, B17)/D$5</f>
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <f>SUMPRODUCT($B$4, B17)/E$5</f>
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <f>SUMPRODUCT($B$5, B17)/F$5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="B17" s="2">
+        <v>-100</v>
+      </c>
+      <c r="D17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="1">
+        <f>SUMPRODUCT($B$3, B17)/E$5</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <f>SUMPRODUCT($B$4, B17)/F$5</f>
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <f>SUMPRODUCT($B$5, B17)/G$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>29</v>
       </c>
-      <c r="D18">
-        <f>SUMPRODUCT($B$3, B18)/D$5</f>
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <f>SUMPRODUCT($B$4, B18)/E$5</f>
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <f>SUMPRODUCT($B$5, B18)/F$5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="B18" s="2">
+        <v>-100</v>
+      </c>
+      <c r="D18" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="1">
+        <f>SUMPRODUCT($B$3, B18)/E$5</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <f>SUMPRODUCT($B$4, B18)/F$5</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <f>SUMPRODUCT($B$5, B18)/G$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>30</v>
       </c>
-      <c r="D19">
-        <f>SUMPRODUCT($B$3, B19)/D$5</f>
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <f>SUMPRODUCT($B$4, B19)/E$5</f>
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <f>SUMPRODUCT($B$5, B19)/F$5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="B19" s="2">
+        <v>-100</v>
+      </c>
+      <c r="D19" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="1">
+        <f>SUMPRODUCT($B$3, B19)/E$5</f>
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <f>SUMPRODUCT($B$4, B19)/F$5</f>
+        <v>0</v>
+      </c>
+      <c r="G19" s="1">
+        <f>SUMPRODUCT($B$5, B19)/G$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>31</v>
       </c>
-      <c r="D20">
-        <f>SUMPRODUCT($B$3, B20)/D$5</f>
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <f>SUMPRODUCT($B$4, B20)/E$5</f>
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <f>SUMPRODUCT($B$5, B20)/F$5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="B20" s="2">
+        <v>-100</v>
+      </c>
+      <c r="D20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="1">
+        <f>SUMPRODUCT($B$3, B20)/E$5</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <f>SUMPRODUCT($B$4, B20)/F$5</f>
+        <v>0</v>
+      </c>
+      <c r="G20" s="1">
+        <f>SUMPRODUCT($B$5, B20)/G$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>32</v>
       </c>
-      <c r="D21">
-        <f>SUMPRODUCT($B$3, B21)/D$5</f>
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <f>SUMPRODUCT($B$4, B21)/E$5</f>
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <f>SUMPRODUCT($B$5, B21)/F$5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="B21" s="2">
+        <v>-100</v>
+      </c>
+      <c r="D21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="1">
+        <f>SUMPRODUCT($B$3, B21)/E$5</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="1">
+        <f>SUMPRODUCT($B$4, B21)/F$5</f>
+        <v>0</v>
+      </c>
+      <c r="G21" s="1">
+        <f>SUMPRODUCT($B$5, B21)/G$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>33</v>
       </c>
-      <c r="D22">
-        <f>SUMPRODUCT($B$3, B22)/D$5</f>
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <f>SUMPRODUCT($B$4, B22)/E$5</f>
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <f>SUMPRODUCT($B$5, B22)/F$5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="B22" s="2">
+        <v>-100</v>
+      </c>
+      <c r="D22" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" s="1">
+        <f>SUMPRODUCT($B$3, B22)/E$5</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="1">
+        <f>SUMPRODUCT($B$4, B22)/F$5</f>
+        <v>0</v>
+      </c>
+      <c r="G22" s="1">
+        <f>SUMPRODUCT($B$5, B22)/G$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>34</v>
       </c>
-      <c r="D23">
-        <f>SUMPRODUCT($B$3, B23)/D$5</f>
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <f>SUMPRODUCT($B$4, B23)/E$5</f>
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <f>SUMPRODUCT($B$5, B23)/F$5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="B23" s="2">
+        <v>-100</v>
+      </c>
+      <c r="D23" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="1">
+        <f>SUMPRODUCT($B$3, B23)/E$5</f>
+        <v>0</v>
+      </c>
+      <c r="F23" s="1">
+        <f>SUMPRODUCT($B$4, B23)/F$5</f>
+        <v>0</v>
+      </c>
+      <c r="G23" s="1">
+        <f>SUMPRODUCT($B$5, B23)/G$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>35</v>
       </c>
-      <c r="D24">
-        <f>SUMPRODUCT($B$3, B24)/D$5</f>
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <f>SUMPRODUCT($B$4, B24)/E$5</f>
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <f>SUMPRODUCT($B$5, B24)/F$5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="B24" s="2">
+        <v>-100</v>
+      </c>
+      <c r="D24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" s="1">
+        <f>SUMPRODUCT($B$3, B24)/E$5</f>
+        <v>0</v>
+      </c>
+      <c r="F24" s="1">
+        <f>SUMPRODUCT($B$4, B24)/F$5</f>
+        <v>0</v>
+      </c>
+      <c r="G24" s="1">
+        <f>SUMPRODUCT($B$5, B24)/G$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>36</v>
       </c>
-      <c r="D25">
-        <f>SUMPRODUCT($B$3, B25)/D$5</f>
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <f>SUMPRODUCT($B$4, B25)/E$5</f>
-        <v>0</v>
-      </c>
-      <c r="F25">
-        <f>SUMPRODUCT($B$5, B25)/F$5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="B25" s="2">
+        <v>-100</v>
+      </c>
+      <c r="D25" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="1">
+        <f>SUMPRODUCT($B$3, B25)/E$5</f>
+        <v>0</v>
+      </c>
+      <c r="F25" s="1">
+        <f>SUMPRODUCT($B$4, B25)/F$5</f>
+        <v>0</v>
+      </c>
+      <c r="G25" s="1">
+        <f>SUMPRODUCT($B$5, B25)/G$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>37</v>
       </c>
-      <c r="D26">
-        <f>SUMPRODUCT($B$3, B26)/D$5</f>
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <f>SUMPRODUCT($B$4, B26)/E$5</f>
-        <v>0</v>
-      </c>
-      <c r="F26">
-        <f>SUMPRODUCT($B$5, B26)/F$5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="B26" s="2">
+        <v>-100</v>
+      </c>
+      <c r="D26" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" s="1">
+        <f>SUMPRODUCT($B$3, B26)/E$5</f>
+        <v>0</v>
+      </c>
+      <c r="F26" s="1">
+        <f>SUMPRODUCT($B$4, B26)/F$5</f>
+        <v>0</v>
+      </c>
+      <c r="G26" s="1">
+        <f>SUMPRODUCT($B$5, B26)/G$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>38</v>
       </c>
-      <c r="D27">
-        <f>SUMPRODUCT($B$3, B27)/D$5</f>
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <f>SUMPRODUCT($B$4, B27)/E$5</f>
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <f>SUMPRODUCT($B$5, B27)/F$5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="B27" s="2">
+        <v>-100</v>
+      </c>
+      <c r="D27" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" s="1">
+        <f>SUMPRODUCT($B$3, B27)/E$5</f>
+        <v>0</v>
+      </c>
+      <c r="F27" s="1">
+        <f>SUMPRODUCT($B$4, B27)/F$5</f>
+        <v>0</v>
+      </c>
+      <c r="G27" s="1">
+        <f>SUMPRODUCT($B$5, B27)/G$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>39</v>
       </c>
-      <c r="D28">
-        <f>SUMPRODUCT($B$3, B28)/D$5</f>
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <f>SUMPRODUCT($B$4, B28)/E$5</f>
-        <v>0</v>
-      </c>
-      <c r="F28">
-        <f>SUMPRODUCT($B$5, B28)/F$5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="B28" s="2">
+        <v>-100</v>
+      </c>
+      <c r="D28" t="s">
+        <v>39</v>
+      </c>
+      <c r="E28" s="1">
+        <f>SUMPRODUCT($B$3, B28)/E$5</f>
+        <v>0</v>
+      </c>
+      <c r="F28" s="1">
+        <f>SUMPRODUCT($B$4, B28)/F$5</f>
+        <v>0</v>
+      </c>
+      <c r="G28" s="1">
+        <f>SUMPRODUCT($B$5, B28)/G$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>40</v>
       </c>
-      <c r="D29">
-        <f>SUMPRODUCT($B$3, B29)/D$5</f>
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <f>SUMPRODUCT($B$4, B29)/E$5</f>
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <f>SUMPRODUCT($B$5, B29)/F$5</f>
+      <c r="B29" s="2">
+        <v>-100</v>
+      </c>
+      <c r="D29" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" s="1">
+        <f>SUMPRODUCT($B$3, B29)/E$5</f>
+        <v>0</v>
+      </c>
+      <c r="F29" s="1">
+        <f>SUMPRODUCT($B$4, B29)/F$5</f>
+        <v>0</v>
+      </c>
+      <c r="G29" s="1">
+        <f>SUMPRODUCT($B$5, B29)/G$5</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E7:G29">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
+      <formula>-100.0</formula>
+      <formula>3.945</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update expected output of big dump
</commit_message>
<xml_diff>
--- a/example_files/dump_of_all_notes.xlsx
+++ b/example_files/dump_of_all_notes.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="43">
   <si>
     <t>Date</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>S2</t>
+  </si>
+  <si>
+    <t>Rounded Notes</t>
   </si>
   <si>
     <t>EOY</t>
@@ -499,13 +502,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -516,7 +519,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -527,7 +530,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -538,7 +541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -549,7 +552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -571,8 +574,11 @@
         <f>IF(SUM($B$5:$C$5)&gt;0,SUM($B$5:$C$5),1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="J5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="F6" t="s">
         <v>13</v>
       </c>
@@ -583,10 +589,16 @@
         <v>15</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>14</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -612,11 +624,19 @@
         <v>0</v>
       </c>
       <c r="J7" s="1">
-        <f>ROUND(AVERAGE(ROUND(G7*10)/10, ROUND(H7*10)/10)*10)/10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <f>ROUND(G7*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
+        <f>ROUND(H7*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
+        <f>ROUND(AVERAGE(J7,K7)*10)/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -642,11 +662,19 @@
         <v>0</v>
       </c>
       <c r="J8" s="1">
-        <f>ROUND(AVERAGE(ROUND(G8*10)/10, ROUND(H8*10)/10)*10)/10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+        <f>ROUND(G8*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
+        <f>ROUND(H8*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
+        <f>ROUND(AVERAGE(J8,K8)*10)/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -672,11 +700,19 @@
         <v>0</v>
       </c>
       <c r="J9" s="1">
-        <f>ROUND(AVERAGE(ROUND(G9*10)/10, ROUND(H9*10)/10)*10)/10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+        <f>ROUND(G9*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
+        <f>ROUND(H9*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
+        <f>ROUND(AVERAGE(J9,K9)*10)/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -702,7 +738,15 @@
         <v>0</v>
       </c>
       <c r="J10" s="1">
-        <f>ROUND(AVERAGE(ROUND(G10*10)/10, ROUND(H10*10)/10)*10)/10</f>
+        <f>ROUND(G10*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="1">
+        <f>ROUND(H10*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="L10" s="1">
+        <f>ROUND(AVERAGE(J10,K10)*10)/10</f>
         <v>0</v>
       </c>
     </row>
@@ -713,7 +757,7 @@
       <formula>3.945</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J7:J10">
+  <conditionalFormatting sqref="J7:L10">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="between">
       <formula>-100.0</formula>
       <formula>3.945</formula>
@@ -725,29 +769,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -755,7 +799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -763,7 +807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -782,8 +826,11 @@
         <f>IF(SUM($B$5)&gt;0,SUM($B$5),1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="I5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="E6" t="s">
         <v>13</v>
       </c>
@@ -794,18 +841,24 @@
         <v>15</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>14</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2">
         <v>-100</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E7" s="1">
         <f>SUMPRODUCT($B$3, B7)/E$5</f>
@@ -820,19 +873,27 @@
         <v>0</v>
       </c>
       <c r="I7" s="1">
-        <f>ROUND(AVERAGE(ROUND(F7*10)/10, ROUND(G7*10)/10)*10)/10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <f>ROUND(F7*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <f>ROUND(G7*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
+        <f>ROUND(AVERAGE(I7,J7)*10)/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B8" s="2">
         <v>-100</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E8" s="1">
         <f>SUMPRODUCT($B$3, B8)/E$5</f>
@@ -847,19 +908,27 @@
         <v>0</v>
       </c>
       <c r="I8" s="1">
-        <f>ROUND(AVERAGE(ROUND(F8*10)/10, ROUND(G8*10)/10)*10)/10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <f>ROUND(F8*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <f>ROUND(G8*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
+        <f>ROUND(AVERAGE(I8,J8)*10)/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B9" s="2">
         <v>-100</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E9" s="1">
         <f>SUMPRODUCT($B$3, B9)/E$5</f>
@@ -874,19 +943,27 @@
         <v>0</v>
       </c>
       <c r="I9" s="1">
-        <f>ROUND(AVERAGE(ROUND(F9*10)/10, ROUND(G9*10)/10)*10)/10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <f>ROUND(F9*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="1">
+        <f>ROUND(G9*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
+        <f>ROUND(AVERAGE(I9,J9)*10)/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B10" s="2">
         <v>-100</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E10" s="1">
         <f>SUMPRODUCT($B$3, B10)/E$5</f>
@@ -901,19 +978,27 @@
         <v>0</v>
       </c>
       <c r="I10" s="1">
-        <f>ROUND(AVERAGE(ROUND(F10*10)/10, ROUND(G10*10)/10)*10)/10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <f>ROUND(F10*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
+        <f>ROUND(G10*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="1">
+        <f>ROUND(AVERAGE(I10,J10)*10)/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B11" s="2">
         <v>-100</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E11" s="1">
         <f>SUMPRODUCT($B$3, B11)/E$5</f>
@@ -928,19 +1013,27 @@
         <v>0</v>
       </c>
       <c r="I11" s="1">
-        <f>ROUND(AVERAGE(ROUND(F11*10)/10, ROUND(G11*10)/10)*10)/10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <f>ROUND(F11*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="1">
+        <f>ROUND(G11*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="1">
+        <f>ROUND(AVERAGE(I11,J11)*10)/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B12" s="2">
         <v>-100</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E12" s="1">
         <f>SUMPRODUCT($B$3, B12)/E$5</f>
@@ -955,19 +1048,27 @@
         <v>0</v>
       </c>
       <c r="I12" s="1">
-        <f>ROUND(AVERAGE(ROUND(F12*10)/10, ROUND(G12*10)/10)*10)/10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <f>ROUND(F12*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="J12" s="1">
+        <f>ROUND(G12*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="1">
+        <f>ROUND(AVERAGE(I12,J12)*10)/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B13" s="2">
         <v>-100</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E13" s="1">
         <f>SUMPRODUCT($B$3, B13)/E$5</f>
@@ -982,19 +1083,27 @@
         <v>0</v>
       </c>
       <c r="I13" s="1">
-        <f>ROUND(AVERAGE(ROUND(F13*10)/10, ROUND(G13*10)/10)*10)/10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <f>ROUND(F13*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="J13" s="1">
+        <f>ROUND(G13*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="1">
+        <f>ROUND(AVERAGE(I13,J13)*10)/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B14" s="2">
         <v>-100</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E14" s="1">
         <f>SUMPRODUCT($B$3, B14)/E$5</f>
@@ -1009,19 +1118,27 @@
         <v>0</v>
       </c>
       <c r="I14" s="1">
-        <f>ROUND(AVERAGE(ROUND(F14*10)/10, ROUND(G14*10)/10)*10)/10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+        <f>ROUND(F14*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="J14" s="1">
+        <f>ROUND(G14*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="K14" s="1">
+        <f>ROUND(AVERAGE(I14,J14)*10)/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B15" s="2">
         <v>-100</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E15" s="1">
         <f>SUMPRODUCT($B$3, B15)/E$5</f>
@@ -1036,19 +1153,27 @@
         <v>0</v>
       </c>
       <c r="I15" s="1">
-        <f>ROUND(AVERAGE(ROUND(F15*10)/10, ROUND(G15*10)/10)*10)/10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+        <f>ROUND(F15*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="J15" s="1">
+        <f>ROUND(G15*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="K15" s="1">
+        <f>ROUND(AVERAGE(I15,J15)*10)/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B16" s="2">
         <v>-100</v>
       </c>
       <c r="D16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E16" s="1">
         <f>SUMPRODUCT($B$3, B16)/E$5</f>
@@ -1063,19 +1188,27 @@
         <v>0</v>
       </c>
       <c r="I16" s="1">
-        <f>ROUND(AVERAGE(ROUND(F16*10)/10, ROUND(G16*10)/10)*10)/10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+        <f>ROUND(F16*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="J16" s="1">
+        <f>ROUND(G16*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="K16" s="1">
+        <f>ROUND(AVERAGE(I16,J16)*10)/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B17" s="2">
         <v>-100</v>
       </c>
       <c r="D17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E17" s="1">
         <f>SUMPRODUCT($B$3, B17)/E$5</f>
@@ -1090,19 +1223,27 @@
         <v>0</v>
       </c>
       <c r="I17" s="1">
-        <f>ROUND(AVERAGE(ROUND(F17*10)/10, ROUND(G17*10)/10)*10)/10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+        <f>ROUND(F17*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="J17" s="1">
+        <f>ROUND(G17*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="K17" s="1">
+        <f>ROUND(AVERAGE(I17,J17)*10)/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B18" s="2">
         <v>-100</v>
       </c>
       <c r="D18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E18" s="1">
         <f>SUMPRODUCT($B$3, B18)/E$5</f>
@@ -1117,19 +1258,27 @@
         <v>0</v>
       </c>
       <c r="I18" s="1">
-        <f>ROUND(AVERAGE(ROUND(F18*10)/10, ROUND(G18*10)/10)*10)/10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+        <f>ROUND(F18*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="J18" s="1">
+        <f>ROUND(G18*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="K18" s="1">
+        <f>ROUND(AVERAGE(I18,J18)*10)/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B19" s="2">
         <v>-100</v>
       </c>
       <c r="D19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E19" s="1">
         <f>SUMPRODUCT($B$3, B19)/E$5</f>
@@ -1144,19 +1293,27 @@
         <v>0</v>
       </c>
       <c r="I19" s="1">
-        <f>ROUND(AVERAGE(ROUND(F19*10)/10, ROUND(G19*10)/10)*10)/10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+        <f>ROUND(F19*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="J19" s="1">
+        <f>ROUND(G19*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="K19" s="1">
+        <f>ROUND(AVERAGE(I19,J19)*10)/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B20" s="2">
         <v>-100</v>
       </c>
       <c r="D20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E20" s="1">
         <f>SUMPRODUCT($B$3, B20)/E$5</f>
@@ -1171,19 +1328,27 @@
         <v>0</v>
       </c>
       <c r="I20" s="1">
-        <f>ROUND(AVERAGE(ROUND(F20*10)/10, ROUND(G20*10)/10)*10)/10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+        <f>ROUND(F20*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="J20" s="1">
+        <f>ROUND(G20*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="K20" s="1">
+        <f>ROUND(AVERAGE(I20,J20)*10)/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B21" s="2">
         <v>-100</v>
       </c>
       <c r="D21" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E21" s="1">
         <f>SUMPRODUCT($B$3, B21)/E$5</f>
@@ -1198,19 +1363,27 @@
         <v>0</v>
       </c>
       <c r="I21" s="1">
-        <f>ROUND(AVERAGE(ROUND(F21*10)/10, ROUND(G21*10)/10)*10)/10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+        <f>ROUND(F21*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="J21" s="1">
+        <f>ROUND(G21*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="K21" s="1">
+        <f>ROUND(AVERAGE(I21,J21)*10)/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B22" s="2">
         <v>-100</v>
       </c>
       <c r="D22" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E22" s="1">
         <f>SUMPRODUCT($B$3, B22)/E$5</f>
@@ -1225,19 +1398,27 @@
         <v>0</v>
       </c>
       <c r="I22" s="1">
-        <f>ROUND(AVERAGE(ROUND(F22*10)/10, ROUND(G22*10)/10)*10)/10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
+        <f>ROUND(F22*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="J22" s="1">
+        <f>ROUND(G22*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="K22" s="1">
+        <f>ROUND(AVERAGE(I22,J22)*10)/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B23" s="2">
         <v>-100</v>
       </c>
       <c r="D23" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E23" s="1">
         <f>SUMPRODUCT($B$3, B23)/E$5</f>
@@ -1252,19 +1433,27 @@
         <v>0</v>
       </c>
       <c r="I23" s="1">
-        <f>ROUND(AVERAGE(ROUND(F23*10)/10, ROUND(G23*10)/10)*10)/10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
+        <f>ROUND(F23*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="J23" s="1">
+        <f>ROUND(G23*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="K23" s="1">
+        <f>ROUND(AVERAGE(I23,J23)*10)/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B24" s="2">
         <v>-100</v>
       </c>
       <c r="D24" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E24" s="1">
         <f>SUMPRODUCT($B$3, B24)/E$5</f>
@@ -1279,19 +1468,27 @@
         <v>0</v>
       </c>
       <c r="I24" s="1">
-        <f>ROUND(AVERAGE(ROUND(F24*10)/10, ROUND(G24*10)/10)*10)/10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+        <f>ROUND(F24*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="J24" s="1">
+        <f>ROUND(G24*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="K24" s="1">
+        <f>ROUND(AVERAGE(I24,J24)*10)/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B25" s="2">
         <v>-100</v>
       </c>
       <c r="D25" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E25" s="1">
         <f>SUMPRODUCT($B$3, B25)/E$5</f>
@@ -1306,19 +1503,27 @@
         <v>0</v>
       </c>
       <c r="I25" s="1">
-        <f>ROUND(AVERAGE(ROUND(F25*10)/10, ROUND(G25*10)/10)*10)/10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
+        <f>ROUND(F25*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="J25" s="1">
+        <f>ROUND(G25*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="K25" s="1">
+        <f>ROUND(AVERAGE(I25,J25)*10)/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B26" s="2">
         <v>-100</v>
       </c>
       <c r="D26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E26" s="1">
         <f>SUMPRODUCT($B$3, B26)/E$5</f>
@@ -1333,19 +1538,27 @@
         <v>0</v>
       </c>
       <c r="I26" s="1">
-        <f>ROUND(AVERAGE(ROUND(F26*10)/10, ROUND(G26*10)/10)*10)/10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
+        <f>ROUND(F26*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="J26" s="1">
+        <f>ROUND(G26*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="K26" s="1">
+        <f>ROUND(AVERAGE(I26,J26)*10)/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B27" s="2">
         <v>-100</v>
       </c>
       <c r="D27" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E27" s="1">
         <f>SUMPRODUCT($B$3, B27)/E$5</f>
@@ -1360,19 +1573,27 @@
         <v>0</v>
       </c>
       <c r="I27" s="1">
-        <f>ROUND(AVERAGE(ROUND(F27*10)/10, ROUND(G27*10)/10)*10)/10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
+        <f>ROUND(F27*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="J27" s="1">
+        <f>ROUND(G27*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="K27" s="1">
+        <f>ROUND(AVERAGE(I27,J27)*10)/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B28" s="2">
         <v>-100</v>
       </c>
       <c r="D28" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E28" s="1">
         <f>SUMPRODUCT($B$3, B28)/E$5</f>
@@ -1387,19 +1608,27 @@
         <v>0</v>
       </c>
       <c r="I28" s="1">
-        <f>ROUND(AVERAGE(ROUND(F28*10)/10, ROUND(G28*10)/10)*10)/10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
+        <f>ROUND(F28*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="J28" s="1">
+        <f>ROUND(G28*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="K28" s="1">
+        <f>ROUND(AVERAGE(I28,J28)*10)/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
       <c r="A29" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B29" s="2">
         <v>-100</v>
       </c>
       <c r="D29" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E29" s="1">
         <f>SUMPRODUCT($B$3, B29)/E$5</f>
@@ -1414,7 +1643,15 @@
         <v>0</v>
       </c>
       <c r="I29" s="1">
-        <f>ROUND(AVERAGE(ROUND(F29*10)/10, ROUND(G29*10)/10)*10)/10</f>
+        <f>ROUND(F29*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="J29" s="1">
+        <f>ROUND(G29*10)/10</f>
+        <v>0</v>
+      </c>
+      <c r="K29" s="1">
+        <f>ROUND(AVERAGE(I29,J29)*10)/10</f>
         <v>0</v>
       </c>
     </row>
@@ -1425,7 +1662,7 @@
       <formula>3.945</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:I29">
+  <conditionalFormatting sqref="I7:K29">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="between">
       <formula>-100.0</formula>
       <formula>3.945</formula>

</xml_diff>